<commit_message>
Changes from call on 20210405
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-PADI-PACPComposition.xlsx
+++ b/output/StructureDefinition-PADI-PACPComposition.xlsx
@@ -1494,7 +1494,7 @@
 &lt;/valueCodeableConcept&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(http://hl7.org/fhir/us/pacio-adi/StructureDefinition/PADI-POLSTObservation|http://hl7.org/fhir/us/pacio-adi/StructureDefinition/PADI-PersonalPrioritiesOrganizer)
+    <t xml:space="preserve">Reference(http://hl7.org/fhir/us/pacio-adi/StructureDefinition/PADI-PersonalInterventionPreference|http://hl7.org/fhir/us/pacio-adi/StructureDefinition/PADI-PersonalPrioritiesOrganizer|http://hl7.org/fhir/us/pacio-adi/StructureDefinition/PADI-PMOLSTObservation)
 </t>
   </si>
   <si>
@@ -1509,7 +1509,7 @@
 &lt;/valueCodeableConcept&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(http://hl7.org/fhir/us/pacio-adi/StructureDefinition/PADI-AutopsyObservation|http://hl7.org/fhir/us/pacio-adi/StructureDefinition/PADI-OrganDonationObservation)
+    <t xml:space="preserve">Reference(http://hl7.org/fhir/us/pacio-adi/StructureDefinition/PADI-PersonalInterventionPreference|http://hl7.org/fhir/us/pacio-adi/StructureDefinition/PADI-PersonalPrioritiesOrganizer|http://hl7.org/fhir/us/pacio-adi/StructureDefinition/PADI-AutopsyObservation|http://hl7.org/fhir/us/pacio-adi/StructureDefinition/PADI-OrganDonationObservation)
 </t>
   </si>
   <si>

</xml_diff>